<commit_message>
Download Excel Data - Parallel_Filter_Stats.xlsx
</commit_message>
<xml_diff>
--- a/datasets/Parallel_Filter_Stats.xlsx
+++ b/datasets/Parallel_Filter_Stats.xlsx
@@ -14,27 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>index</t>
   </si>
   <si>
-    <t>POX/C</t>
-  </si>
-  <si>
-    <t>C/A</t>
-  </si>
-  <si>
-    <t>POX/M</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>PDI</t>
-  </si>
-  <si>
-    <t>Mn</t>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>MashTime</t>
+  </si>
+  <si>
+    <t>SolidosFermentaveis</t>
+  </si>
+  <si>
+    <t>SolidosNaoFermentaveis</t>
+  </si>
+  <si>
+    <t>SolidosTotais</t>
+  </si>
+  <si>
+    <t>PercFermentaveis</t>
+  </si>
+  <si>
+    <t>Extrato</t>
+  </si>
+  <si>
+    <t>MashingEfficiency</t>
+  </si>
+  <si>
+    <t>Dp1</t>
+  </si>
+  <si>
+    <t>Dp2</t>
+  </si>
+  <si>
+    <t>Dp3</t>
+  </si>
+  <si>
+    <t>Dp4Plus</t>
   </si>
   <si>
     <t>count</t>
@@ -416,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,189 +462,351 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C2">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="D2">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E2">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="F2">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="G2">
-        <v>5000</v>
+        <v>1000</v>
+      </c>
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>1000</v>
+      </c>
+      <c r="K2">
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>1000</v>
+      </c>
+      <c r="M2">
+        <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>100.6333726210634</v>
+        <v>65</v>
       </c>
       <c r="C3">
-        <v>0.09925941260153906</v>
+        <v>100</v>
       </c>
       <c r="D3">
-        <v>0.001000158844475234</v>
+        <v>96.94092994264039</v>
       </c>
       <c r="E3">
-        <v>0.7129116607825223</v>
+        <v>48.49040226979136</v>
       </c>
       <c r="F3">
-        <v>1.032834501503651</v>
+        <v>152.4615906654977</v>
       </c>
       <c r="G3">
-        <v>78679.42036668859</v>
+        <v>63.47926899177205</v>
+      </c>
+      <c r="H3">
+        <v>14.54313322124318</v>
+      </c>
+      <c r="I3">
+        <v>95.29886035261634</v>
+      </c>
+      <c r="J3">
+        <v>7.913637169029514</v>
+      </c>
+      <c r="K3">
+        <v>45.49775780026358</v>
+      </c>
+      <c r="L3">
+        <v>10.06787402247895</v>
+      </c>
+      <c r="M3">
+        <v>31.81959136084431</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>5.336630602724714</v>
+        <v>9.998494677726423</v>
       </c>
       <c r="C4">
-        <v>0.005307434109865392</v>
+        <v>29.99548403317927</v>
       </c>
       <c r="D4">
-        <v>5.415584578606771E-05</v>
+        <v>22.09488519857674</v>
       </c>
       <c r="E4">
-        <v>0.01258091392606887</v>
+        <v>13.31724655041774</v>
       </c>
       <c r="F4">
-        <v>0.0008582535715661018</v>
+        <v>1.123328699128405</v>
       </c>
       <c r="G4">
-        <v>3954.211204650129</v>
+        <v>14.22205674278546</v>
+      </c>
+      <c r="H4">
+        <v>2.275842876167337</v>
+      </c>
+      <c r="I4">
+        <v>14.6476119442378</v>
+      </c>
+      <c r="J4">
+        <v>1.250674003895388</v>
+      </c>
+      <c r="K4">
+        <v>12.80693754054486</v>
+      </c>
+      <c r="L4">
+        <v>2.075530562340822</v>
+      </c>
+      <c r="M4">
+        <v>8.867311140844556</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>80.40036015459947</v>
+        <v>32.09473268508106</v>
       </c>
       <c r="C5">
-        <v>0.08040036015459946</v>
+        <v>1.284198055243166</v>
       </c>
       <c r="D5">
-        <v>0.0008040036015459947</v>
+        <v>15.50705457086778</v>
       </c>
       <c r="E5">
-        <v>0.6589070971454469</v>
+        <v>13.59428172819732</v>
       </c>
       <c r="F5">
-        <v>1.030699840299889</v>
+        <v>148.10697344438</v>
       </c>
       <c r="G5">
-        <v>66385.94263255737</v>
+        <v>10.4701718023367</v>
+      </c>
+      <c r="H5">
+        <v>3.600697344437997</v>
+      </c>
+      <c r="I5">
+        <v>24.31146394190683</v>
+      </c>
+      <c r="J5">
+        <v>3.46254299624347</v>
+      </c>
+      <c r="K5">
+        <v>7.00762880609323</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>9.150886220158162</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>97.03580126111225</v>
+        <v>58.26296131778599</v>
       </c>
       <c r="C6">
-        <v>0.09568128549757383</v>
+        <v>79.78888395335795</v>
       </c>
       <c r="D6">
-        <v>0.000963634818538748</v>
+        <v>89.73933244461371</v>
       </c>
       <c r="E6">
-        <v>0.7047652903117418</v>
+        <v>40.11173855912033</v>
       </c>
       <c r="F6">
-        <v>1.032226631245835</v>
+        <v>152.163736052687</v>
       </c>
       <c r="G6">
-        <v>75895.82389142229</v>
+        <v>58.98729052204998</v>
+      </c>
+      <c r="H6">
+        <v>15.15110282411983</v>
+      </c>
+      <c r="I6">
+        <v>99.64800337717145</v>
+      </c>
+      <c r="J6">
+        <v>7.199932893177007</v>
+      </c>
+      <c r="K6">
+        <v>39.58943849195545</v>
+      </c>
+      <c r="L6">
+        <v>10.6950767294104</v>
+      </c>
+      <c r="M6">
+        <v>26.20262024773336</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>100.6340729774889</v>
+        <v>65</v>
       </c>
       <c r="C7">
-        <v>0.09925926583316903</v>
+        <v>100</v>
       </c>
       <c r="D7">
-        <v>0.001000157451887214</v>
+        <v>105.8768879966164</v>
       </c>
       <c r="E7">
-        <v>0.7128604072133971</v>
+        <v>44.86397495528115</v>
       </c>
       <c r="F7">
-        <v>1.032737860401861</v>
+        <v>152.9140553288643</v>
       </c>
       <c r="G7">
-        <v>78565.22485624734</v>
+        <v>69.23879595889238</v>
+      </c>
+      <c r="H7">
+        <v>15.28698364340404</v>
+      </c>
+      <c r="I7">
+        <v>99.99916469286694</v>
+      </c>
+      <c r="J7">
+        <v>7.670735716254943</v>
+      </c>
+      <c r="K7">
+        <v>50.65271883845252</v>
+      </c>
+      <c r="L7">
+        <v>10.70235330613033</v>
+      </c>
+      <c r="M7">
+        <v>29.34608123116248</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>104.2318845832973</v>
+        <v>71.73703868221402</v>
       </c>
       <c r="C8">
-        <v>0.102837901791626</v>
+        <v>120.211116046642</v>
       </c>
       <c r="D8">
-        <v>0.001036696591716831</v>
+        <v>112.2942878222007</v>
       </c>
       <c r="E8">
-        <v>0.721285434918427</v>
+        <v>51.42766546338035</v>
       </c>
       <c r="F8">
-        <v>1.033355202078378</v>
+        <v>153.2103440366889</v>
       </c>
       <c r="G8">
-        <v>81263.30362759363</v>
+        <v>73.29419466744451</v>
+      </c>
+      <c r="H8">
+        <v>15.32053653781785</v>
+      </c>
+      <c r="I8">
+        <v>99.99999586186635</v>
+      </c>
+      <c r="J8">
+        <v>8.316078059309714</v>
+      </c>
+      <c r="K8">
+        <v>55.29412598582952</v>
+      </c>
+      <c r="L8">
+        <v>10.72136415644584</v>
+      </c>
+      <c r="M8">
+        <v>33.72328583140195</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B9">
-        <v>119.5996398454005</v>
+        <v>97.90526731491926</v>
       </c>
       <c r="C9">
-        <v>0.1195996398454005</v>
+        <v>198.7158019447578</v>
       </c>
       <c r="D9">
-        <v>0.001195996398454005</v>
+        <v>114.5695897190051</v>
       </c>
       <c r="E9">
-        <v>0.7662818102089913</v>
+        <v>85.74294277731047</v>
       </c>
       <c r="F9">
-        <v>1.037885298125204</v>
+        <v>153.3148027818198</v>
       </c>
       <c r="G9">
-        <v>94500.7072118778</v>
+        <v>74.7283286676809</v>
+      </c>
+      <c r="H9">
+        <v>15.33148027346516</v>
+      </c>
+      <c r="I9">
+        <v>99.99999999996247</v>
+      </c>
+      <c r="J9">
+        <v>10.74933242774137</v>
+      </c>
+      <c r="K9">
+        <v>56.95111272001579</v>
+      </c>
+      <c r="L9">
+        <v>10.79451731378597</v>
+      </c>
+      <c r="M9">
+        <v>57.03254907861945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>